<commit_message>
adding the bold, font dynamic control
</commit_message>
<xml_diff>
--- a/public/data/hymns_collection.xlsx
+++ b/public/data/hymns_collection.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800"/>
+    <workbookView windowWidth="19200" windowHeight="6080" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Songs" sheetId="1" r:id="rId1"/>
+    <sheet name="Only Believe Song Book" sheetId="1" r:id="rId1"/>
+    <sheet name="Icilongo" sheetId="2" r:id="rId2"/>
+    <sheet name="Difelo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27934,7 +27936,7 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -28628,8 +28630,8 @@
   <sheetPr/>
   <dimension ref="A1:E1086"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="A2:D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -47107,4 +47109,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>